<commit_message>
Update tableau de compétence
</commit_message>
<xml_diff>
--- a/files/skill.xlsx
+++ b/files/skill.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilian\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ilian\Desktop\inecer.github.io\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7BBAD-850A-4ACA-8EA4-36942009DEBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1195C76-3A92-4D88-9F5D-F02570D0F075}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -140,9 +140,6 @@
     <t>23/05/2022 au 27/06/2022</t>
   </si>
   <si>
-    <t>Oui</t>
-  </si>
-  <si>
     <t>☑ SISR</t>
   </si>
   <si>
@@ -150,6 +147,9 @@
   </si>
   <si>
     <t>Adresse URL du portfolio : https://inecer.github.io/</t>
+  </si>
+  <si>
+    <t>✘</t>
   </si>
 </sst>
 </file>
@@ -678,9 +678,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -704,51 +749,6 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1094,8 +1094,8 @@
   </sheetPr>
   <dimension ref="A1:AQ81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="76" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="76" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.81640625" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1108,83 +1108,83 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="H1" s="21"/>
+      <c r="H1" s="25"/>
     </row>
     <row r="2" spans="1:43" ht="41" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="21" t="s">
+      <c r="A2" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
+      <c r="B2" s="25"/>
+      <c r="C2" s="25"/>
+      <c r="D2" s="25"/>
+      <c r="E2" s="25"/>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="24"/>
-      <c r="F3" s="28" t="s">
+      <c r="A3" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="38"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="29"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="44"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
     </row>
     <row r="4" spans="1:43" ht="40" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="26"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="27"/>
+      <c r="B4" s="41"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="42"/>
       <c r="F4" s="14" t="s">
         <v>8</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="20" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:43" ht="40" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="40" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" s="41"/>
-      <c r="C5" s="41"/>
-      <c r="D5" s="41"/>
-      <c r="E5" s="41"/>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="42"/>
+      <c r="A5" s="34" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:43" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="38" t="s">
+      <c r="B6" s="32" t="s">
         <v>19</v>
       </c>
       <c r="C6" s="6" t="s">
@@ -1207,8 +1207,8 @@
       </c>
     </row>
     <row r="7" spans="1:43" s="2" customFormat="1" ht="325" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="31"/>
-      <c r="B7" s="39"/>
+      <c r="A7" s="24"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="8" t="s">
         <v>9</v>
       </c>
@@ -1264,16 +1264,16 @@
       <c r="AQ7"/>
     </row>
     <row r="8" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A8" s="32" t="s">
+      <c r="A8" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="33"/>
-      <c r="C8" s="33"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="33"/>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="28"/>
       <c r="I8"/>
       <c r="J8"/>
       <c r="K8"/>
@@ -1314,24 +1314,24 @@
       <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="43" t="s">
+      <c r="B9" s="21" t="s">
         <v>28</v>
       </c>
       <c r="C9" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D9" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E9" s="16"/>
       <c r="F9" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G9" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H9" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I9"/>
       <c r="J9"/>
@@ -1377,20 +1377,20 @@
         <v>29</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D10" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E10" s="16"/>
       <c r="F10" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G10" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H10" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I10"/>
       <c r="J10"/>
@@ -1432,22 +1432,22 @@
       <c r="A11" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="22" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D11" s="16"/>
       <c r="E11" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H11" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I11"/>
       <c r="J11"/>
@@ -1489,24 +1489,24 @@
       <c r="A12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C12" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D12" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="E12" s="16"/>
       <c r="F12" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="G12" s="16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I12"/>
       <c r="J12"/>
@@ -1815,16 +1815,16 @@
       <c r="AQ18"/>
     </row>
     <row r="19" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A19" s="35" t="s">
+      <c r="A19" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="36"/>
-      <c r="F19" s="36"/>
-      <c r="G19" s="36"/>
-      <c r="H19" s="37"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="31"/>
       <c r="I19"/>
       <c r="J19"/>
       <c r="K19"/>
@@ -2177,16 +2177,16 @@
       <c r="AQ26"/>
     </row>
     <row r="27" spans="1:43" s="2" customFormat="1" ht="18" x14ac:dyDescent="0.25">
-      <c r="A27" s="35" t="s">
+      <c r="A27" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="37"/>
+      <c r="B27" s="30"/>
+      <c r="C27" s="30"/>
+      <c r="D27" s="30"/>
+      <c r="E27" s="30"/>
+      <c r="F27" s="30"/>
+      <c r="G27" s="30"/>
+      <c r="H27" s="31"/>
       <c r="I27"/>
       <c r="J27"/>
       <c r="K27"/>
@@ -2631,6 +2631,11 @@
     <row r="81" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A4:E4"/>
+    <mergeCell ref="F3:H3"/>
     <mergeCell ref="A6:A7"/>
     <mergeCell ref="A2:H2"/>
     <mergeCell ref="A8:H8"/>
@@ -2638,11 +2643,6 @@
     <mergeCell ref="A27:H27"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="A5:H5"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A4:E4"/>
-    <mergeCell ref="F3:H3"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>